<commit_message>
Aggiornati file data e reprot
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ITSVIL00000/I.T. Svil Srl/4Heasy ADT/v.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ITSVIL00000/I.T. Svil Srl/4Heasy ADT/v.1.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabat\Desktop\A1#111ITSVIL00000\I.T. Svil Srl\4Heasy ADT\v.1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2A6DC4-3608-4F51-87AB-5B8A97F78807}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2531D5-EFB0-4AFC-BB0A-D61B1996F658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,15 +623,6 @@
     <t>Errore semantico</t>
   </si>
   <si>
-    <t>2025-07-01T16:34:43Z</t>
-  </si>
-  <si>
-    <t>d468db7f8cfe8bda73886ee8b1413c33</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.303de62cc2fb651db3ef78bd94842ad093f6293b7c77a989c8db069b1a684e86.90865f0b70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>55c752ad88238050ff5fd46754ddecd7</t>
   </si>
   <si>
@@ -669,24 +660,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.70103.4.6.303de62cc2fb651db3ef78bd94842ad093f6293b7c77a989c8db069b1a684e86.4e0f3cdf9d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-07-01T16:34:52Z</t>
-  </si>
-  <si>
-    <t>21b67aa9e0b600a30c0711c213f9ac9d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.303de62cc2fb651db3ef78bd94842ad093f6293b7c77a989c8db069b1a684e86.1041854244^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-07-01T16:34:54Z</t>
-  </si>
-  <si>
-    <t>4cd6122c6dd3526f2afc65e4027d7fb0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70103.4.6.303de62cc2fb651db3ef78bd94842ad093f6293b7c77a989c8db069b1a684e86.ae4cc6dc19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_LDO_TIMEOUT</t>
@@ -732,6 +705,33 @@
   </si>
   <si>
     <t>Tempo massimo della richiesta scaduto riprovare</t>
+  </si>
+  <si>
+    <t>2025-07-07T10:30:57Z</t>
+  </si>
+  <si>
+    <t>2ba992d7db365ecbbe49fe1d677c40ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.59a1cccfeb2481c41f2ac36a2949dbd4e8c14576af16f39365e34cc8afadc427.6d268c3e0c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-07-07T10:31:04Z</t>
+  </si>
+  <si>
+    <t>2025-07-07T10:31:06Z</t>
+  </si>
+  <si>
+    <t>871900ef167362e71ff3f4b84ec79069</t>
+  </si>
+  <si>
+    <t>fa814b73952bd66c54d4acb1fb2617ec</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.59a1cccfeb2481c41f2ac36a2949dbd4e8c14576af16f39365e34cc8afadc427.fc61f914de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70103.4.6.59a1cccfeb2481c41f2ac36a2949dbd4e8c14576af16f39365e34cc8afadc427.ee0f9f695a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2787,10 +2787,10 @@
   <dimension ref="A1:W584"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="N19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3214,10 +3214,10 @@
         <v>37</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F12" s="34">
         <v>45839</v>
@@ -3237,7 +3237,7 @@
         <v>49</v>
       </c>
       <c r="O12" s="35" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="P12" s="35" t="s">
         <v>49</v>
@@ -3342,16 +3342,16 @@
         <v>86</v>
       </c>
       <c r="F14" s="34">
-        <v>45839</v>
+        <v>45845</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="I14" s="39" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="J14" s="35" t="s">
         <v>49</v>
@@ -3408,13 +3408,13 @@
         <v>45839</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J15" s="35" t="s">
         <v>49</v>
@@ -3471,13 +3471,13 @@
         <v>45839</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I16" s="39" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J16" s="35" t="s">
         <v>49</v>
@@ -3491,7 +3491,7 @@
         <v>49</v>
       </c>
       <c r="O16" s="35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P16" s="35" t="s">
         <v>49</v>
@@ -3525,10 +3525,10 @@
         <v>37</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -3575,13 +3575,13 @@
         <v>45839</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I18" s="39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J18" s="35" t="s">
         <v>49</v>
@@ -3629,10 +3629,10 @@
         <v>37</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
@@ -3670,10 +3670,10 @@
         <v>37</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -3720,13 +3720,13 @@
         <v>45839</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I21" s="39" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J21" s="35" t="s">
         <v>49</v>
@@ -3740,7 +3740,7 @@
         <v>49</v>
       </c>
       <c r="O21" s="35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P21" s="35" t="s">
         <v>49</v>
@@ -3774,10 +3774,10 @@
         <v>37</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -3821,16 +3821,16 @@
         <v>98</v>
       </c>
       <c r="F23" s="34">
-        <v>45839</v>
+        <v>45845</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="I23" s="39" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="J23" s="35" t="s">
         <v>49</v>
@@ -3870,16 +3870,16 @@
         <v>99</v>
       </c>
       <c r="F24" s="34">
-        <v>45839</v>
+        <v>45845</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="I24" s="39" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="J24" s="35" t="s">
         <v>49</v>
@@ -3913,10 +3913,10 @@
         <v>37</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
@@ -10230,15 +10230,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10496,6 +10487,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10509,14 +10509,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10531,6 +10523,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>